<commit_message>
Added some reports and figures
</commit_message>
<xml_diff>
--- a/Sensors_Comprehensive.xlsx
+++ b/Sensors_Comprehensive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Desktop\2018 Ubuntu Shared\GitShared\Ratiometric_Microscopy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28624881-6909-4C4F-9CAE-34BB8FCEB253}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DCF0B3-3617-4513-B888-B66C24CBA49E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="1" xr2:uid="{C64352C4-4D56-4B65-AB60-CCCFC1A3AD62}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" xr2:uid="{C64352C4-4D56-4B65-AB60-CCCFC1A3AD62}"/>
   </bookViews>
   <sheets>
     <sheet name="Redox" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
     <t>Sensor</t>
   </si>
@@ -132,18 +132,12 @@
     <t>roGFP1-iL</t>
   </si>
   <si>
-    <t>roGFP1-iX</t>
-  </si>
-  <si>
     <t>roGFP2-iL</t>
   </si>
   <si>
     <t>Grx1-roGFP2</t>
   </si>
   <si>
-    <t>Estimates based on Gutscher 2008, figure S3</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -151,6 +145,105 @@
   </si>
   <si>
     <t>Romero2014</t>
+  </si>
+  <si>
+    <t>pHRed</t>
+  </si>
+  <si>
+    <t>mKeima</t>
+  </si>
+  <si>
+    <t>pKa</t>
+  </si>
+  <si>
+    <t>CannonThesisPg26</t>
+  </si>
+  <si>
+    <t>Cannon thesis shows roGFP1-R9 spectra, but doesn't claim that the curves are limiting. Maybe we can infer based on dynamic range?</t>
+  </si>
+  <si>
+    <t>deGFP1</t>
+  </si>
+  <si>
+    <t>deGFP2</t>
+  </si>
+  <si>
+    <t>HansonThesisPg52</t>
+  </si>
+  <si>
+    <t>HansonThesisPg53</t>
+  </si>
+  <si>
+    <t>deGFP4</t>
+  </si>
+  <si>
+    <t>deGFP3</t>
+  </si>
+  <si>
+    <t>More information Hanson Thesis Pg. 70</t>
+  </si>
+  <si>
+    <t>HansonThesisPg94</t>
+  </si>
+  <si>
+    <t>HansonThesisPg95</t>
+  </si>
+  <si>
+    <t>HansonThesisPg103</t>
+  </si>
+  <si>
+    <t>HansonThesisPg104</t>
+  </si>
+  <si>
+    <t>roGFP1-iQ</t>
+  </si>
+  <si>
+    <t>roGFP1-iH</t>
+  </si>
+  <si>
+    <t>roGFP1-iR</t>
+  </si>
+  <si>
+    <t>roGFP1-iS</t>
+  </si>
+  <si>
+    <t>roGFP1-iD</t>
+  </si>
+  <si>
+    <t>Midpoint Confidence (+/-)</t>
+  </si>
+  <si>
+    <t>Reported dyanmic range of 4.5 @ 400/503</t>
+  </si>
+  <si>
+    <t>LohamThesisPg24</t>
+  </si>
+  <si>
+    <t>Number of spectra</t>
+  </si>
+  <si>
+    <t>Estimates based on Gutscher 2008, figure S3. Midpoint was -291 at pH 7 and -315 at pH 7.4, Shokhina 2019.</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Spectra Collected</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>neg 320 and 230 mv</t>
+  </si>
+  <si>
+    <t>neg 310 and 230 mv</t>
+  </si>
+  <si>
+    <t>neg 330 and 240 mv</t>
+  </si>
+  <si>
+    <t>neg 330 and 250 mv</t>
   </si>
 </sst>
 </file>
@@ -158,7 +251,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -177,12 +270,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -197,11 +296,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,26 +628,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C263D91-C584-420E-B573-414262512C57}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="84" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="84" style="5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -552,25 +666,31 @@
         <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -586,135 +706,222 @@
       <c r="E2">
         <v>-281</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>6.5</v>
       </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
       <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7">
         <v>-269</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7">
         <v>5.6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7">
         <v>-282</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
         <v>-268</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7">
         <v>6.2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E6">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
         <v>-284</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7">
         <v>7.5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E7">
         <v>-278</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>7.2</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="M7" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
         <v>-284</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
         <v>6.2</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E9">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7">
         <v>-275</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7">
         <v>5.4</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E10">
         <v>-265</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>5.6</v>
       </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
       <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -730,177 +937,420 @@
       <c r="E11">
         <v>-265</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <f>C11/B11</f>
         <v>7.8065967016491751</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E12">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7">
         <v>-263</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7">
         <v>5.6</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7">
+        <v>-229</v>
+      </c>
+      <c r="F13" s="7">
+        <v>5</v>
+      </c>
+      <c r="G13" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1.07</v>
-      </c>
-      <c r="C15">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2">
+        <f>1.07 / 1.25</f>
+        <v>0.85600000000000009</v>
+      </c>
+      <c r="C14">
+        <f>3.1 * 1.25</f>
+        <v>3.875</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <v>-236</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14" s="1">
+        <f>C14/B14</f>
+        <v>4.5268691588785046</v>
+      </c>
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7">
+        <v>-239</v>
+      </c>
+      <c r="F15" s="7">
+        <v>6</v>
+      </c>
+      <c r="G15" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7">
+        <v>-238</v>
+      </c>
+      <c r="F16" s="7">
+        <v>4</v>
+      </c>
+      <c r="G16" s="10">
         <v>3.1</v>
       </c>
-      <c r="D15">
-        <v>0.5</v>
-      </c>
-      <c r="E15">
-        <v>-236</v>
-      </c>
-      <c r="F15" s="1">
-        <f>C15/B15</f>
-        <v>2.8971962616822431</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="H16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7">
+        <v>-237</v>
+      </c>
+      <c r="F17" s="7">
+        <v>5</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2.9</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7">
+        <v>-240</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2.4</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7">
+        <v>-246</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="10">
+        <v>2.8</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B20">
         <v>0.09</v>
       </c>
-      <c r="C16">
+      <c r="C20">
         <v>1.7</v>
       </c>
-      <c r="D16">
+      <c r="D20">
         <v>0.3</v>
       </c>
-      <c r="E16">
+      <c r="E20">
         <v>-272</v>
       </c>
-      <c r="F16">
+      <c r="G20">
         <v>5.8</v>
       </c>
-      <c r="G16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="1">
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1">
         <f>15500/45000</f>
         <v>0.34444444444444444</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C21" s="1">
         <f>47000/23000</f>
         <v>2.0434782608695654</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D21" s="1">
         <f>23/45</f>
         <v>0.51111111111111107</v>
       </c>
-      <c r="E17">
+      <c r="E21">
         <v>-272</v>
       </c>
-      <c r="F17" s="1">
-        <f>C17/B17</f>
+      <c r="G21" s="1">
+        <f>C21/B21</f>
         <v>5.9326788218793833</v>
       </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18">
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
         <v>0.19</v>
       </c>
-      <c r="C18">
+      <c r="C22">
         <v>0.45</v>
       </c>
-      <c r="D18">
+      <c r="D22">
         <v>0.65</v>
       </c>
-      <c r="E18">
+      <c r="E22">
         <v>-229</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E19">
+      <c r="E23">
         <v>-299</v>
       </c>
-      <c r="F19">
+      <c r="G23">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E20">
+      <c r="E24">
         <v>-286</v>
       </c>
-      <c r="F20">
+      <c r="G24">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E21">
+      <c r="E25">
         <v>-296</v>
       </c>
-      <c r="F21">
+      <c r="G25">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="H25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" t="s">
+        <v>53</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E22">
+      <c r="E26">
         <v>-280</v>
       </c>
-      <c r="F22">
+      <c r="G26">
         <v>5.4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>51</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27">
+        <f>COUNTIF(H2:H26, "Yes")</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -911,13 +1361,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDB5626-33EF-459E-AADB-B66D7A7B4BCF}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -933,7 +1390,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>19</v>
@@ -952,6 +1409,101 @@
       </c>
       <c r="K1" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>0.16</v>
+      </c>
+      <c r="C2">
+        <v>5.83</v>
+      </c>
+      <c r="D2">
+        <v>0.16</v>
+      </c>
+      <c r="E2">
+        <v>7.8</v>
+      </c>
+      <c r="F2">
+        <f>C2/B2</f>
+        <v>36.4375</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>0.73</v>
+      </c>
+      <c r="C3">
+        <v>22.41</v>
+      </c>
+      <c r="D3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E3">
+        <v>6.6</v>
+      </c>
+      <c r="F3">
+        <f>C3/B3</f>
+        <v>30.698630136986303</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4">
+        <v>7.8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>